<commit_message>
update a lot of thing
</commit_message>
<xml_diff>
--- a/.FileQuanTrong/22-23/TKB-HK2-22-23.xlsx
+++ b/.FileQuanTrong/22-23/TKB-HK2-22-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\SGU-Course\.FileQuanTrong\22-23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835652BD-E6F5-4E3B-8A5A-CE92BC909893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16351EF7-31E5-4343-8EFB-C81C2D943AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,19 +121,26 @@
     <t>QP IV</t>
   </si>
   <si>
-    <t>T.T.Khoa</t>
+    <t>T.T.Nhã</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -401,14 +408,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -417,97 +424,100 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -787,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D10:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -822,10 +832,12 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="28" t="s">
+      <c r="I11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="1"/>
+      <c r="J11" s="20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="4:10" ht="15.75">
       <c r="D12" s="9">
@@ -834,9 +846,11 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="1"/>
+      <c r="H12" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12" s="21"/>
     </row>
     <row r="13" spans="4:10" ht="15.75">
       <c r="D13" s="9">
@@ -845,46 +859,46 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="1"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="17" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="4:10" ht="15.75">
       <c r="D14" s="9">
         <v>4</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="31" t="s">
+      <c r="F14" s="1"/>
+      <c r="G14" s="20" t="s">
         <v>25</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="J14" s="18"/>
     </row>
     <row r="15" spans="4:10" ht="15.75">
       <c r="D15" s="9">
         <v>5</v>
       </c>
       <c r="E15" s="1"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="21"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="4:10" ht="15.75">
       <c r="D16" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
     </row>
     <row r="17" spans="4:11" ht="15.75">
       <c r="D17" s="9">
@@ -892,13 +906,11 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="28" t="s">
+      <c r="H17" s="1"/>
+      <c r="I17" s="17" t="s">
         <v>28</v>
       </c>
       <c r="J17" s="1"/>
@@ -910,8 +922,8 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="33"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="29"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="18"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="4:11" ht="15.75">
@@ -919,14 +931,12 @@
         <v>8</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="1"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="29"/>
+      <c r="I19" s="18"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="4:11" ht="15.75">
@@ -934,10 +944,10 @@
         <v>9</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="33"/>
+      <c r="F20" s="1"/>
       <c r="G20" s="33"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="30"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="19"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="4:11" ht="15.75">
@@ -945,9 +955,9 @@
         <v>10</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="30"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
@@ -963,15 +973,15 @@
       <c r="E25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19" t="s">
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="J25" s="19"/>
+      <c r="J25" s="35"/>
     </row>
     <row r="26" spans="4:11">
       <c r="D26" s="10">
@@ -980,12 +990,12 @@
       <c r="E26" s="6">
         <v>1</v>
       </c>
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
-      <c r="I26" s="27" t="s">
+      <c r="I26" s="15" t="s">
         <v>14</v>
       </c>
       <c r="J26" s="25"/>
@@ -998,14 +1008,14 @@
         <v>841407</v>
       </c>
       <c r="E27" s="6">
-        <v>3</v>
-      </c>
-      <c r="F27" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="13" t="s">
         <v>16</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
-      <c r="I27" s="27" t="s">
+      <c r="I27" s="36" t="s">
         <v>29</v>
       </c>
       <c r="J27" s="25"/>
@@ -1020,12 +1030,12 @@
       <c r="E28" s="6">
         <v>4</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G28" s="24"/>
       <c r="H28" s="24"/>
-      <c r="I28" s="27" t="s">
+      <c r="I28" s="15" t="s">
         <v>19</v>
       </c>
       <c r="J28" s="25"/>
@@ -1038,17 +1048,17 @@
         <v>841110</v>
       </c>
       <c r="E29" s="11">
-        <v>1</v>
-      </c>
-      <c r="F29" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="27" t="s">
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="J29" s="21"/>
+      <c r="J29" s="16"/>
       <c r="K29" s="12">
         <v>4</v>
       </c>
@@ -1060,15 +1070,15 @@
       <c r="E30" s="11">
         <v>3</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="F30" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="27" t="s">
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J30" s="21"/>
+      <c r="J30" s="16"/>
       <c r="K30" s="12">
         <v>2</v>
       </c>
@@ -1080,15 +1090,15 @@
       <c r="E31" s="6">
         <v>2</v>
       </c>
-      <c r="F31" s="34" t="s">
+      <c r="F31" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="G31" s="14"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="35" t="s">
+      <c r="G31" s="27"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="J31" s="17"/>
+      <c r="J31" s="30"/>
       <c r="K31">
         <v>4</v>
       </c>
@@ -1096,20 +1106,20 @@
     <row r="32" spans="4:11">
       <c r="D32" s="5"/>
       <c r="E32" s="6"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="17"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="30"/>
     </row>
     <row r="33" spans="4:11">
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="17"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="30"/>
     </row>
     <row r="34" spans="4:11">
       <c r="K34">
@@ -1130,15 +1140,7 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="G17:G21"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="I11:I13"/>
     <mergeCell ref="H19:H21"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="I17:I20"/>
     <mergeCell ref="D36:J36"/>
     <mergeCell ref="F26:H26"/>
     <mergeCell ref="I26:J26"/>
@@ -1146,18 +1148,26 @@
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="I27:J27"/>
-    <mergeCell ref="H17:H18"/>
     <mergeCell ref="F32:H32"/>
     <mergeCell ref="I32:J32"/>
     <mergeCell ref="F33:H33"/>
     <mergeCell ref="I33:J33"/>
-    <mergeCell ref="E16:J16"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="I28:J28"/>
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="F30:H30"/>
     <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I17:I20"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="E16:J16"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="H12:H13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>